<commit_message>
Actualización de catálogo y promociones
</commit_message>
<xml_diff>
--- a/data/catalogo.xlsx
+++ b/data/catalogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infob\Desktop\JQ_Motors_web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BE6789-6EED-4070-A60B-12EA09F8FDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFD2E5E-4BB7-4B5C-A47E-D8F660591058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4620" yWindow="2655" windowWidth="14430" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11120,8 +11120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>